<commit_message>
24x crank and fan speed fix
</commit_message>
<xml_diff>
--- a/EngineController_Rev2/Wiring/20200920_1987ChevyImpala_ECUPinout.xlsx
+++ b/EngineController_Rev2/Wiring/20200920_1987ChevyImpala_ECUPinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxar\Documents\GitHub\Fischers-Bullshit\EngineController_Rev2\Wiring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90214C43-BCAE-4775-8467-1CC845A26B56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F180668-C1E1-4E36-A266-0DCD18942A7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="869" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IO summary" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,6 @@
   <customWorkbookViews>
     <customWorkbookView name="Gordan Jurasek - Personal View" guid="{42220FEB-052A-431B-AE3E-56BDD95FF573}" autoUpdate="1" mergeInterval="10" personalView="1" maximized="1" windowWidth="743" windowHeight="620" activeSheetId="1"/>
   </customWorkbookViews>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2596,8 +2595,8 @@
   </sheetPr>
   <dimension ref="A1:K474"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -10735,8 +10734,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10847,7 +10846,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11931,7 +11930,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13996,7 +13995,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14739,21 +14738,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010069BE6D43D67CEB43AED07C7F7D5C5717" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed3a72aebdc31f7dceab7adc1698e9d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7dcf5c17-6cdd-4fc8-89b5-5b1e79518785" xmlns:ns3="d00a5386-c7cb-4c27-81c4-161dee80d926" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13c9d8c14350f29f3105e6e4a5c07352" ns2:_="" ns3:_="">
     <xsd:import namespace="7dcf5c17-6cdd-4fc8-89b5-5b1e79518785"/>
@@ -14948,10 +14932,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40107F8D-B0B7-4341-9E98-865C53748BD9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24A5A8A-4F4A-4C73-89E8-8A0B9B9754E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7dcf5c17-6cdd-4fc8-89b5-5b1e79518785"/>
+    <ds:schemaRef ds:uri="d00a5386-c7cb-4c27-81c4-161dee80d926"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14974,20 +14984,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24A5A8A-4F4A-4C73-89E8-8A0B9B9754E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40107F8D-B0B7-4341-9E98-865C53748BD9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7dcf5c17-6cdd-4fc8-89b5-5b1e79518785"/>
-    <ds:schemaRef ds:uri="d00a5386-c7cb-4c27-81c4-161dee80d926"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>